<commit_message>
Map path fixes made during the meeting with Sean
</commit_message>
<xml_diff>
--- a/PDigyExample.xlsx
+++ b/PDigyExample.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/osahin/Projects/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/osahin/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8524DDC6-BB82-E343-B2EA-4D5E07857A53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E4EE5F3-5525-E641-ABFD-A713A0B873D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5740" yWindow="10700" windowWidth="30240" windowHeight="18880" xr2:uid="{66416868-3D12-A547-BAF1-AFD683643788}"/>
+    <workbookView xWindow="-33920" yWindow="-20240" windowWidth="51200" windowHeight="28300" xr2:uid="{66416868-3D12-A547-BAF1-AFD683643788}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Code</t>
   </si>
@@ -61,6 +61,12 @@
   </si>
   <si>
     <t xml:space="preserve">{"calibrate0","sharpen"} </t>
+  </si>
+  <si>
+    <t>"015"</t>
+  </si>
+  <si>
+    <t>"F"</t>
   </si>
 </sst>
 </file>
@@ -429,8 +435,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DD997CC-1478-8242-9FBD-FF04F973818F}">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" zoomScale="329" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -488,6 +494,14 @@
         <v>11</v>
       </c>
     </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+    </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
     </row>

</xml_diff>